<commit_message>
+inventaris, +bp titel, extra screens
</commit_message>
<xml_diff>
--- a/documentatie/gegevens/inventaris.xlsx
+++ b/documentatie/gegevens/inventaris.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stagair1\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stagair1\Documents\Stage_en_BP_2018\documentatie\gegevens\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="39">
   <si>
     <t>Hardware</t>
   </si>
@@ -65,9 +65,6 @@
     <t>10.1.205.1/16</t>
   </si>
   <si>
-    <t>Virtual AD</t>
-  </si>
-  <si>
     <t>IBM x3650 M3 7945G2G</t>
   </si>
   <si>
@@ -86,9 +83,6 @@
     <t>10.1.205.2/16</t>
   </si>
   <si>
-    <t>Virtual Fileserver</t>
-  </si>
-  <si>
     <t>10.1.205.11/16</t>
   </si>
   <si>
@@ -105,6 +99,48 @@
   </si>
   <si>
     <t>Netscaler Internal</t>
+  </si>
+  <si>
+    <t>10.1.205.10/16</t>
+  </si>
+  <si>
+    <t>Citrix License Server Virtual Appliance v11.14.0.1_19800</t>
+  </si>
+  <si>
+    <t>Virtual License Server</t>
+  </si>
+  <si>
+    <t>Netscaler Management</t>
+  </si>
+  <si>
+    <t>10.1.205.4/16</t>
+  </si>
+  <si>
+    <t>AAA Virtual Server</t>
+  </si>
+  <si>
+    <t>10.1.205.5/16</t>
+  </si>
+  <si>
+    <t>Hostname</t>
+  </si>
+  <si>
+    <t>netscaler</t>
+  </si>
+  <si>
+    <t>ldap</t>
+  </si>
+  <si>
+    <t>Virutal LDAP server</t>
+  </si>
+  <si>
+    <t>Virtual file server</t>
+  </si>
+  <si>
+    <t>fileserver</t>
+  </si>
+  <si>
+    <t>ShareFile</t>
   </si>
 </sst>
 </file>
@@ -444,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -455,14 +491,15 @@
     <col min="1" max="1" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="15.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -473,67 +510,70 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="3">
         <v>2</v>
@@ -542,89 +582,167 @@
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="G4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23"/>
+        <v>17</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24"/>
@@ -634,6 +752,9 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
bp - SSO herschrijven + HSTS
</commit_message>
<xml_diff>
--- a/documentatie/gegevens/inventaris.xlsx
+++ b/documentatie/gegevens/inventaris.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="47">
   <si>
     <t>Hardware</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>fileserver2</t>
+  </si>
+  <si>
+    <t>10.1.205.7/16</t>
   </si>
 </sst>
 </file>
@@ -501,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -681,10 +684,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>5</v>
@@ -693,10 +696,10 @@
         <v>6</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -707,10 +710,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>5</v>
@@ -733,10 +736,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>5</v>
@@ -745,10 +748,10 @@
         <v>6</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -759,10 +762,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>5</v>
@@ -774,7 +777,7 @@
         <v>20</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -782,25 +785,25 @@
         <v>11</v>
       </c>
       <c r="B11" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -811,7 +814,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>32</v>
@@ -826,11 +829,34 @@
         <v>20</v>
       </c>
       <c r="H12" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26"/>
@@ -840,6 +866,9 @@
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>